<commit_message>
fix: jadwal excel import format cell
</commit_message>
<xml_diff>
--- a/public/templates/template_jadwal.xlsx
+++ b/public/templates/template_jadwal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ridzimeko\Documents\Projects\jadwal-azmania\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751B8C35-73CA-4895-A3EB-D659C76483B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8B7B74-96A9-4B71-B1F1-8F460F850283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2865FED8-1D15-40F6-8E78-7F59FD911D5F}"/>
   </bookViews>
@@ -151,12 +151,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -270,14 +273,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90018943-7AD0-4845-8AC9-80DDA7D942A6}" name="Table1" displayName="Table1" ref="A1:E61" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90018943-7AD0-4845-8AC9-80DDA7D942A6}" name="Table1" displayName="Table1" ref="A1:E61" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:E61" xr:uid="{90018943-7AD0-4845-8AC9-80DDA7D942A6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7D525FBE-40AC-47DB-8530-6E9C3B2F11F5}" name="Kode Kelas" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{AC690FDF-2941-4E30-9672-D0FEA9C2F73B}" name="Kode Mata Pelajaran" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{BA978D68-9475-42B3-B100-80A7C9B8F004}" name="Kode Guru Pengajar"/>
+    <tableColumn id="1" xr3:uid="{7D525FBE-40AC-47DB-8530-6E9C3B2F11F5}" name="Kode Kelas" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{AC690FDF-2941-4E30-9672-D0FEA9C2F73B}" name="Kode Mata Pelajaran" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{BA978D68-9475-42B3-B100-80A7C9B8F004}" name="Kode Guru Pengajar" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{D1E7D42B-2E9F-491C-B453-3F034819E37D}" name="Hari"/>
-    <tableColumn id="3" xr3:uid="{E1E49A4B-CA51-40BE-A1BE-F0C1980A29A8}" name="Jam Ke" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{E1E49A4B-CA51-40BE-A1BE-F0C1980A29A8}" name="Jam Ke" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -580,17 +583,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8C8015-952B-497B-B9AD-00108CB18956}">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22" style="3" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
@@ -600,10 +603,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -687,147 +690,6 @@
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="3"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="3"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="3"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="3"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="3"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="3"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
fix(excel): format cell jadwal
</commit_message>
<xml_diff>
--- a/public/templates/template_jadwal.xlsx
+++ b/public/templates/template_jadwal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ridzimeko\Documents\Projects\jadwal-azmania\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8B7B74-96A9-4B71-B1F1-8F460F850283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A67E14-0FB1-487B-898B-6FEC0563D4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2865FED8-1D15-40F6-8E78-7F59FD911D5F}"/>
   </bookViews>
@@ -77,10 +77,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
-    <numFmt numFmtId="165" formatCode="[$-13809]hh:mm;@"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,14 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -159,7 +152,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -277,10 +270,10 @@
   <autoFilter ref="A1:E61" xr:uid="{90018943-7AD0-4845-8AC9-80DDA7D942A6}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{7D525FBE-40AC-47DB-8530-6E9C3B2F11F5}" name="Kode Kelas" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{AC690FDF-2941-4E30-9672-D0FEA9C2F73B}" name="Kode Mata Pelajaran" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{AC690FDF-2941-4E30-9672-D0FEA9C2F73B}" name="Kode Mata Pelajaran" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{BA978D68-9475-42B3-B100-80A7C9B8F004}" name="Kode Guru Pengajar" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{D1E7D42B-2E9F-491C-B453-3F034819E37D}" name="Hari"/>
-    <tableColumn id="3" xr3:uid="{E1E49A4B-CA51-40BE-A1BE-F0C1980A29A8}" name="Jam Ke" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{E1E49A4B-CA51-40BE-A1BE-F0C1980A29A8}" name="Jam Ke" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -586,7 +579,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +588,7 @@
     <col min="2" max="2" width="26.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="22" style="3" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -612,84 +605,81 @@
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E2" s="6"/>
-    </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -725,7 +715,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>